<commit_message>
keep metadata as dataframe
</commit_message>
<xml_diff>
--- a/slic3roptions.xlsx
+++ b/slic3roptions.xlsx
@@ -1183,8 +1183,8 @@
   </sheetPr>
   <dimension ref="A1:E144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>